<commit_message>
Tuning material_05: The second important variable becomes the first
</commit_message>
<xml_diff>
--- a/github/workflows/Hyein/multkan_sweep_autosave/CrossedBarrel_20251229_1531.xlsx
+++ b/github/workflows/Hyein/multkan_sweep_autosave/CrossedBarrel_20251229_1531.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD72"/>
+  <dimension ref="A1:AD77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8154,486 +8154,229 @@
         </is>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AA2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>val_loss</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>train_loss</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>test_loss</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>r2_train</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>r2_val</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>r2_test</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>seed</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>device</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>spline_train_loss</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>spline_test_loss</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>param_width</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>param_grid_range</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>param_grid</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>param_k</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>param_mult_arity</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>param_steps</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>param_opt</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>param_lr</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>param_update_grid</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>param_lamb</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>param_lamb_coef</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>param_lamb_entropy</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>param_prune</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>param_pruning_node_th</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>param_pruning_edge_th</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>param_symbolic</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>param_sym_weight_simple</t>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>0.4742208902376184</v>
+      </c>
+      <c r="B73" t="n">
+        <v>0.4642983548666572</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0.4656494662123681</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0.1032185852527618</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.1061024069786072</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0.1040449216961861</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0.1067662239074707</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0.1116792112588882</v>
+      </c>
+      <c r="I73" t="n">
+        <v>1</v>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr"/>
+      <c r="L73" t="inlineStr"/>
+      <c r="M73" t="inlineStr"/>
+      <c r="N73" t="n">
+        <v>30</v>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>[0.1, 0.9]</t>
+        </is>
+      </c>
+      <c r="P73" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q73" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="R73" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="S73" t="n">
+        <v>1</v>
+      </c>
+      <c r="T73" t="n">
+        <v>1</v>
+      </c>
+      <c r="U73" t="n">
+        <v>0</v>
+      </c>
+      <c r="V73" t="inlineStr">
+        <is>
+          <t>LBFGS</t>
+        </is>
+      </c>
+      <c r="W73" t="b">
+        <v>1</v>
+      </c>
+      <c r="X73" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="Y73" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Z73" t="n">
+        <v>50</v>
+      </c>
+      <c r="AA73" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB73" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC73" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD73" t="inlineStr">
+        <is>
+          <t>[[4, 0], [4, 0], [1, 0]]</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>0.08803174644708633</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0.0832786038517952</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.08839752525091171</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.6359443556812205</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.6217614203905578</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.5824614520616311</v>
-      </c>
-      <c r="G2" t="n">
-        <v>8</v>
-      </c>
-      <c r="H2" t="inlineStr">
+    <row r="74">
+      <c r="A74" t="n">
+        <v>0.5542138134777302</v>
+      </c>
+      <c r="B74" t="n">
+        <v>0.5105522791542797</v>
+      </c>
+      <c r="C74" t="n">
+        <v>0.5662840536867609</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0.09139586240053177</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0.0969061553478241</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.09093237668275833</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0.1024894714355469</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0.1101778596639633</v>
+      </c>
+      <c r="I74" t="n">
+        <v>2</v>
+      </c>
+      <c r="J74" t="inlineStr">
         <is>
           <t>cpu</t>
         </is>
       </c>
-      <c r="I2" t="n">
-        <v>0.1022694334387779</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.1133446097373962</v>
-      </c>
-      <c r="K2" t="inlineStr">
+      <c r="K74" t="inlineStr"/>
+      <c r="L74" t="inlineStr"/>
+      <c r="M74" t="inlineStr"/>
+      <c r="N74" t="n">
+        <v>30</v>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>[0.1, 0.9]</t>
+        </is>
+      </c>
+      <c r="P74" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q74" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="R74" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="S74" t="n">
+        <v>1</v>
+      </c>
+      <c r="T74" t="n">
+        <v>1</v>
+      </c>
+      <c r="U74" t="n">
+        <v>0</v>
+      </c>
+      <c r="V74" t="inlineStr">
+        <is>
+          <t>LBFGS</t>
+        </is>
+      </c>
+      <c r="W74" t="b">
+        <v>1</v>
+      </c>
+      <c r="X74" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="Y74" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Z74" t="n">
+        <v>50</v>
+      </c>
+      <c r="AA74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB74" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC74" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD74" t="inlineStr">
         <is>
           <t>[[4, 0], [4, 0], [1, 0]]</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>[0.1, 0.9]</t>
-        </is>
-      </c>
-      <c r="M2" t="n">
-        <v>30</v>
-      </c>
-      <c r="N2" t="n">
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>-99</v>
+      </c>
+      <c r="B75" t="n">
+        <v>-99</v>
+      </c>
+      <c r="C75" t="n">
+        <v>-99</v>
+      </c>
+      <c r="D75" t="n">
+        <v>999</v>
+      </c>
+      <c r="E75" t="n">
+        <v>999</v>
+      </c>
+      <c r="F75" t="n">
+        <v>999</v>
+      </c>
+      <c r="G75" t="inlineStr"/>
+      <c r="H75" t="inlineStr"/>
+      <c r="I75" t="n">
         <v>3</v>
       </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>50</v>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>LBFGS</t>
-        </is>
-      </c>
-      <c r="R2" t="n">
-        <v>1</v>
-      </c>
-      <c r="S2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T2" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="U2" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="V2" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="W2" t="b">
-        <v>1</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="Z2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>completed</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>total</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>8</v>
-      </c>
-      <c r="B2" t="n">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AB2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>val_loss</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>train_loss</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>test_loss</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>r2_train</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>r2_val</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>r2_test</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>seed</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>device</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>error</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>traceback</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>timestamp</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>param_width</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>param_grid_range</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>param_grid</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>param_k</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>param_mult_arity</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>param_steps</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>param_opt</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>param_lr</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>param_update_grid</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>param_lamb</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>param_lamb_coef</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>param_lamb_entropy</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>param_prune</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>param_pruning_node_th</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>param_pruning_edge_th</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>param_symbolic</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>param_sym_weight_simple</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>999</v>
-      </c>
-      <c r="B2" t="n">
-        <v>999</v>
-      </c>
-      <c r="C2" t="n">
-        <v>999</v>
-      </c>
-      <c r="D2" t="n">
-        <v>-99</v>
-      </c>
-      <c r="E2" t="n">
-        <v>-99</v>
-      </c>
-      <c r="F2" t="n">
-        <v>-99</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="inlineStr">
+      <c r="J75" t="inlineStr">
         <is>
           <t>cpu</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="K75" t="inlineStr">
         <is>
           <t>Failed during symbolification or subsequent fitting/plotting</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="L75" t="inlineStr">
         <is>
           <t xml:space="preserve">Traceback (most recent call last):
   File "D:\pykan\kan\experiments\multkan_hparam_sweep.py", line 231, in _run_single_trial
@@ -8669,66 +8412,787 @@
 </t>
         </is>
       </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>2025-12-29T16:45:15</t>
+        </is>
+      </c>
+      <c r="N75" t="n">
+        <v>30</v>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>[0.1, 0.9]</t>
+        </is>
+      </c>
+      <c r="P75" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q75" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="R75" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="S75" t="n">
+        <v>1</v>
+      </c>
+      <c r="T75" t="n">
+        <v>1</v>
+      </c>
+      <c r="U75" t="n">
+        <v>0</v>
+      </c>
+      <c r="V75" t="inlineStr">
+        <is>
+          <t>LBFGS</t>
+        </is>
+      </c>
+      <c r="W75" t="b">
+        <v>1</v>
+      </c>
+      <c r="X75" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="Y75" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Z75" t="n">
+        <v>50</v>
+      </c>
+      <c r="AA75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB75" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC75" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD75" t="inlineStr">
+        <is>
+          <t>[[4, 0], [4, 0], [1, 0]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>0.5285772591635787</v>
+      </c>
+      <c r="B76" t="n">
+        <v>0.4957378418490037</v>
+      </c>
+      <c r="C76" t="n">
+        <v>0.5320378516820548</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0.09564891457557678</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.09872075170278549</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0.09343606233596802</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0.1076338738203049</v>
+      </c>
+      <c r="H76" t="n">
+        <v>0.1121385544538498</v>
+      </c>
+      <c r="I76" t="n">
+        <v>4</v>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr"/>
+      <c r="L76" t="inlineStr"/>
+      <c r="M76" t="inlineStr"/>
+      <c r="N76" t="n">
+        <v>30</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>[0.1, 0.9]</t>
+        </is>
+      </c>
+      <c r="P76" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q76" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="R76" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="S76" t="n">
+        <v>1</v>
+      </c>
+      <c r="T76" t="n">
+        <v>1</v>
+      </c>
+      <c r="U76" t="n">
+        <v>0</v>
+      </c>
+      <c r="V76" t="inlineStr">
+        <is>
+          <t>LBFGS</t>
+        </is>
+      </c>
+      <c r="W76" t="b">
+        <v>1</v>
+      </c>
+      <c r="X76" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="Y76" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Z76" t="n">
+        <v>50</v>
+      </c>
+      <c r="AA76" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB76" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC76" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD76" t="inlineStr">
+        <is>
+          <t>[[4, 0], [4, 0], [1, 0]]</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>0.5028243444641844</v>
+      </c>
+      <c r="B77" t="n">
+        <v>0.5093113723000617</v>
+      </c>
+      <c r="C77" t="n">
+        <v>0.4606268227925134</v>
+      </c>
+      <c r="D77" t="n">
+        <v>0.1019090265035629</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.1024037897586823</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0.1046876981854439</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0.1015421152114868</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0.1121792644262314</v>
+      </c>
+      <c r="I77" t="n">
+        <v>5</v>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr"/>
+      <c r="L77" t="inlineStr"/>
+      <c r="M77" t="inlineStr"/>
+      <c r="N77" t="n">
+        <v>30</v>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>[0.1, 0.9]</t>
+        </is>
+      </c>
+      <c r="P77" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q77" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="R77" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="S77" t="n">
+        <v>1</v>
+      </c>
+      <c r="T77" t="n">
+        <v>1</v>
+      </c>
+      <c r="U77" t="n">
+        <v>0</v>
+      </c>
+      <c r="V77" t="inlineStr">
+        <is>
+          <t>LBFGS</t>
+        </is>
+      </c>
+      <c r="W77" t="b">
+        <v>1</v>
+      </c>
+      <c r="X77" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="Y77" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Z77" t="n">
+        <v>50</v>
+      </c>
+      <c r="AA77" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB77" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC77" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD77" t="inlineStr">
+        <is>
+          <t>[[4, 0], [4, 0], [1, 0]]</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AA2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>val_loss</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>train_loss</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>test_loss</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>r2_train</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>r2_val</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>r2_test</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>seed</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>device</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>spline_train_loss</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>spline_test_loss</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>param_width</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>param_grid_range</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>param_grid</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>param_k</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>param_mult_arity</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>param_steps</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>param_opt</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>param_lr</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>param_update_grid</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>param_lamb</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>param_lamb_coef</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>param_lamb_entropy</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>param_prune</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>param_pruning_node_th</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>param_pruning_edge_th</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>param_symbolic</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>param_sym_weight_simple</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0.08803174644708633</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.0832786038517952</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.08839752525091171</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.6359443556812205</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.6217614203905578</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.5824614520616311</v>
+      </c>
+      <c r="G2" t="n">
+        <v>8</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>0.1022694334387779</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.1133446097373962</v>
+      </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2025-12-29T16:42:15</t>
+          <t>[[4, 0], [4, 0], [1, 0]]</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
+          <t>[0.1, 0.9]</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>30</v>
+      </c>
+      <c r="N2" t="n">
+        <v>3</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>LBFGS</t>
+        </is>
+      </c>
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="W2" t="b">
+        <v>1</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="Z2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>8</v>
+      </c>
+      <c r="B2" t="n">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AA2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>val_loss</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>train_loss</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>test_loss</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>r2_train</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>r2_val</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>r2_test</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>seed</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>device</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>spline_train_loss</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>spline_test_loss</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>param_width</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>param_grid_range</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>param_grid</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>param_k</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>param_mult_arity</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>param_steps</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>param_opt</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>param_lr</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>param_update_grid</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>param_lamb</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>param_lamb_coef</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>param_lamb_entropy</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>param_prune</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>param_pruning_node_th</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>param_pruning_edge_th</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>param_symbolic</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>param_sym_weight_simple</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0.1024037897586823</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.1019090265035629</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.1046876981854439</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.5028243444641844</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.5093113723000617</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.4606268227925134</v>
+      </c>
+      <c r="G2" t="n">
+        <v>5</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>cpu</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>0.1015421152114868</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.1121792644262314</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
           <t>[[4, 0], [4, 0], [1, 0]]</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>[0.1, 0.9]</t>
         </is>
       </c>
+      <c r="M2" t="n">
+        <v>30</v>
+      </c>
       <c r="N2" t="n">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="O2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="n">
         <v>50</v>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>LBFGS</t>
         </is>
       </c>
-      <c r="S2" t="n">
-        <v>1</v>
-      </c>
-      <c r="T2" t="b">
-        <v>1</v>
+      <c r="R2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.001</v>
       </c>
       <c r="U2" t="n">
-        <v>0.001</v>
+        <v>0.01</v>
       </c>
       <c r="V2" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="W2" t="n">
-        <v>1</v>
-      </c>
-      <c r="X2" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="W2" t="b">
+        <v>1</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.01</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="Z2" t="n">
         <v>0.03</v>
       </c>
-      <c r="AA2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AB2" t="n">
+      <c r="Z2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>